<commit_message>
Updates: plots for ORF, dropout, log10A posteriors; new runs; etc.
</commit_message>
<xml_diff>
--- a/data/dr2_timing_20200607/corr_noise_jobs.xlsx
+++ b/data/dr2_timing_20200607/corr_noise_jobs.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -454,391 +454,255 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>ppta_ptmcmc_ms_gwb_fixsl_infer_orf_set_3_1_ephem_0</t>
+          <t>ppta_ptmcmc_pe_gwb_fixsl_infer_orf_set_x_1_ephem_0</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>/home/bgonchar/correlated_noise_pta_2020/slurm/ppta_dr2_ptmcmc_ms_gwb_fixslope_infer_orf_set_3_1_ephem_0_20201020.sh</t>
+          <t>/home/bgonchar/correlated_noise_pta_2020/slurm/ppta_dr2_ptmcmc_pe_gwb_fixslope_infer_orf_set_x_1_ephem_0_20201022.sh</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>/fred/oz002/bgoncharov/correlated_noise_pta_2020_out/dr2_timing_20200607/20200908_20201020_gwb_fixgamma_varorf_3psr/completed.txt</t>
+          <t>/fred/oz002/bgoncharov/correlated_noise_pta_2020_out/dr2_timing_20200607/20201020_gwb_fixgamma_varorf_x1psr/completed.txt</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>ppta_ptmcmc_ms_gwb_fixsl_infer_orf_set_x_1_ephem_0</t>
+          <t>ppta_ptmcmc_pe_gwb_cpl_fixslope_set_x_1_eph_0</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>/home/bgonchar/correlated_noise_pta_2020/slurm/ppta_dr2_ptmcmc_ms_gwb_fixslope_infer_orf_set_x_1_ephem_0_20201020.sh</t>
+          <t>/home/bgonchar/correlated_noise_pta_2020/slurm/ppta_dr2_ptmcmc_pe_cpl_gwb_fixslope_set_x_1_ephem_0_20201103.sh</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>/fred/oz002/bgoncharov/correlated_noise_pta_2020_out/dr2_timing_20200607/20200908_20201020_gwb_fixgamma_varorf_x1psr/completed.txt</t>
+          <t>/fred/oz002/bgoncharov/correlated_noise_pta_2020_out/dr2_timing_20200607/20200908_cpl_gwb_fixgamma_x1psr/completed.txt</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>ppta_ptmcmc_ms_gwb_fixslope_set_all_ephem_0_ns</t>
+          <t>ppta_ptmcmc_pe_gwb_cpl_fixsl_inforf_set_x_1_eph_0</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>/home/bgonchar/correlated_noise_pta_2020/slurm/ppta_dr2_ptmcmc_ms_gwb_fixslope_set_all_ephem_0_ns_20200928.sh</t>
+          <t>/home/bgonchar/correlated_noise_pta_2020/slurm/ppta_dr2_ptmcmc_pe_gwb_cpl_fixslope_infer_orf_set_x_1_ephem_0_20201030.sh</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>/fred/oz002/bgoncharov/correlated_noise_pta_2020_out/dr2_timing_20200607/20200908_20200908_gwb_fixgamma_allpsr/20200908_20200908_gwb_fixgamma_allpsr_result.json</t>
+          <t>/fred/oz002/bgoncharov/correlated_noise_pta_2020_out/dr2_timing_20200607/20201030_gwb_cpl_fixgamma_varorf_x1psr/completed.txt</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>ppta_ptmcmc_ms_gwb_fixslope_set_x_1_ephem_0</t>
+          <t>ppta_ptmcmc_ms_gwb_cpl_fixslope_set_x_1_ephem_0</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>/home/bgonchar/correlated_noise_pta_2020/slurm/ppta_dr2_ptmcmc_ms_gwb_fixslope_set_x_1_ephem_0_20200928.sh</t>
+          <t>/home/bgonchar/correlated_noise_pta_2020/slurm/ppta_dr2_ptmcmc_ms_cpl_gwb_fixslope_set_x_1_ephem_0_20201027.sh</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>/fred/oz002/bgoncharov/correlated_noise_pta_2020_out/dr2_timing_20200607/20200908_20200908_gwb_fixgamma_x1psr/completed.txt</t>
+          <t>/fred/oz002/bgoncharov/correlated_noise_pta_2020_out/dr2_timing_20200607/20200910_cpl_fixgam_20200908_gwb_fixgamma_x1psr/completed.txt</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>ppta_ptmcmc_ms_gwb_fixslope_set_x_1_ephem_c1</t>
+          <t>ppta_ptmcmc_ms_cpl_gwb_cpl_fixslope_set_x_1_eph_0</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>/home/bgonchar/correlated_noise_pta_2020/slurm/ppta_dr2_ptmcmc_ms_gwb_fixslope_set_x_1_ephem_c1_20201019.sh</t>
+          <t>/home/bgonchar/correlated_noise_pta_2020/slurm/ppta_dr2_ptmcmc_ms_cpl_cpl_gwb_fixslope_set_x_1_ephem_0_20201030.sh</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>/fred/oz002/bgoncharov/correlated_noise_pta_2020_out/dr2_timing_20200607/20200930_be_c1_20201008_gwb_fixgamma_eph_c1_x1psr/completed.txt</t>
+          <t>/fred/oz002/bgoncharov/correlated_noise_pta_2020_out/dr2_timing_20200607/20201030_gwb_fixgamma_namehd_20200908_cpl_gwb_fixgamma_x1psr/completed.txt</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>ppta_nicer_ms_cpl_varslope_set_all_ephem_0</t>
+          <t>ppta_ptmcmc_pe_gwb_fixsl_inter_orf_set_x_1_ephem_0</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>/home/bgonchar/correlated_noise_pta_2020/slurm/ppta_dr2_nicer_ptmcmc_ms_cpl_varslope_set_all_ephem_0_20201008.sh</t>
+          <t>/home/bgonchar/correlated_noise_pta_2020/slurm/ppta_dr2_ptmcmc_pe_gwb_fixslope_interp_orf_set_x_1_ephem_0_20201105.sh</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>/fred/oz002/bgoncharov/correlated_noise_pta_2020_out/dr2_nicer_20201008/20201008_20201008_cpl_vargam_allpsr/completed.txt</t>
+          <t>/fred/oz002/bgoncharov/correlated_noise_pta_2020_out/dr2_timing_20200607/20201020_gwb_fixgamma_interporf_x1psr/completed.txt</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>ppta_ptmcmc_pe_set_x_1_ephem_c1</t>
+          <t>ppta_ptmcmc_pe_gwb_cpl_fixsl_intorf_set_x_1_eph_0</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>/home/bgonchar/correlated_noise_pta_2020/slurm/ppta_dr2_ptmcmc_pe_set_x_1_ephem_c1_20201020.sh</t>
+          <t>/home/bgonchar/correlated_noise_pta_2020/slurm/ppta_dr2_ptmcmc_pe_gwb_cpl_fixslope_interp_orf_set_x_1_ephem_0_20201105.sh</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>/fred/oz002/bgoncharov/correlated_noise_pta_2020_out/dr2_timing_20200607/20200930_be_c1_x1psr/completed.txt</t>
+          <t>/fred/oz002/bgoncharov/correlated_noise_pta_2020_out/dr2_timing_20200607/20201105_gwb_cpl_fixgamma_interporf_x1psr/completed.txt</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>ppta_nicer_pe_set_all_ephem_c1</t>
+          <t>ppta_ptmcmc_pe_gwb_cpl_noa_fixsl_set_x_1_eph_0</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>/home/bgonchar/correlated_noise_pta_2020/slurm/ppta_dr2_nicer_ptmcmc_pe_set_all_ephem_c1_20201014.sh</t>
+          <t>/home/bgonchar/correlated_noise_pta_2020/slurm/ppta_dr2_ptmcmc_pe_cpl_gwb_noauto_fixslope_set_20_nf_x_1_ephem_0_20201109.sh</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>/fred/oz002/bgoncharov/correlated_noise_pta_2020_out/dr2_nicer_20201008/20201008_eph_c1_allpsr/completed.txt</t>
+          <t>/fred/oz002/bgoncharov/correlated_noise_pta_2020_out/dr2_timing_20200607/20200908_cpl_gwb_noa_fixgam_20_nf_x1psr/completed.txt</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>ppta_ptmcmc_pe_cpl_freesp_30_nf_set_3_1_ephem_c1</t>
+          <t>ppta_ptmcmc_pe_gwb_fixsl_inforf_20nf_set_x1_eph_0</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>/home/bgonchar/correlated_noise_pta_2020/slurm/ppta_dr2_ptmcmc_ms_cpl_freesp_30_nf_set_3_1_ephem_c1_20201015.sh</t>
+          <t>/home/bgonchar/correlated_noise_pta_2020/slurm/ppta_dr2_ptmcmc_pe_gwb_fixslope_infer_orf_20_nf_set_x_1_ephem_0_20201111.sh</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>/fred/oz002/bgoncharov/correlated_noise_pta_2020_out/dr2_timing_20200607/20201015_cpl_freesp_30_nf_be_c1_3psr/completed.txt</t>
+          <t>/fred/oz002/bgoncharov/correlated_noise_pta_2020_out/dr2_timing_20200607/20201020_gwb_fixgamma_varorf_20_nf_x1psr/completed.txt</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>ppta_ptmcmc_pe_cpl_freesp_30_nf_set_x_1_ephem_c1</t>
+          <t>ppta_ptmcmc_ms_gwb_cpl_fixsl_20nf_set_x1_eph0</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>/home/bgonchar/correlated_noise_pta_2020/slurm/ppta_dr2_ptmcmc_ms_cpl_freesp_30_nf_set_x_1_ephem_c1_20201015.sh</t>
+          <t>/home/bgonchar/correlated_noise_pta_2020/slurm/ppta_dr2_ptmcmc_ms_cpl_gwb_fixslope_20_nf_set_x_1_ephem_0_20201111.sh</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>/fred/oz002/bgoncharov/correlated_noise_pta_2020_out/dr2_timing_20200607/20201015_cpl_freesp_30_nf_be_c1_x1psr/completed.txt</t>
+          <t>/fred/oz002/bgoncharov/correlated_noise_pta_2020_out/dr2_timing_20200607/20200910_cpl_fixgam_20_nf_20200908_gwb_fixgamma_20_nf_x1psr/completed.txt</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>ppta_nicer_ms_cpl_varslope_set_all_ephem_0_1</t>
+          <t>ppta_ptmcmc_pe_gwb_fixsl_intorf_20nf_setx1_eph0</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>/home/bgonchar/correlated_noise_pta_2020/slurm/ppta_dr2_nicer_ptmcmc_ms_cpl_varslope_set_all_ephem_0_20201015.sh</t>
+          <t>/home/bgonchar/correlated_noise_pta_2020/slurm/ppta_dr2_ptmcmc_pe_gwb_fixslope_interp_orf_20_nf_set_x_1_ephem_0_20201105.sh</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>/fred/oz002/bgoncharov/correlated_noise_pta_2020_out/dr2_nicer_20201008/20201015_20201015_cpl_vargam_allpsr/completed.txt</t>
+          <t>/fred/oz002/bgoncharov/correlated_noise_pta_2020_out/dr2_timing_20200607/20201111_gwb_fixgamma_interporf_20_nf_x1psr/completed.txt</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>ppta_nicer_ptmcmc_pe_singlepsr_freesp_30_nf</t>
+          <t>ppta_ptmcmc_ms_mon_cpl_fixsl_20nf_set_x_1</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>/home/bgonchar/correlated_noise_pta_2020/slurm/ppta_dr2_nicer_ptmcmc_pe_singlepsr_freesp_30_nf_20201020.sh</t>
+          <t>/home/bgonchar/correlated_noise_pta_2020/slurm/ppta_dr2_ptmcmc_ms_cpl_monop_fixslope_20_nf_set_x_1_ephem_0_20201117.sh</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>/fred/oz002/bgoncharov/correlated_noise_pta_2020_out/dr2_nicer_20201008/20201020_cpl_freesp_30_nf_singpsr/0_J0437-4715/NO_SUCH_FILE_JUST_STOP_MANUALLY.txt</t>
+          <t>/fred/oz002/bgoncharov/correlated_noise_pta_2020_out/dr2_timing_20200607/20200910_cpl_fixgam_20_nf_20201117_monop_fixgamma_20_nf_x1psr/completed.txt</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>ppta_ptmcmc_ms_set_x_1_ephem_jup_el_5</t>
+          <t>ppta_ptmcmc_ms_dip_cpl_fixsl_20nf_set_x_1</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>/home/bgonchar/correlated_noise_pta_2020/slurm/ppta_dr2_ptmcmc_ms_set_x_1_jup_el_5_20201021.sh</t>
+          <t>/home/bgonchar/correlated_noise_pta_2020/slurm/ppta_dr2_ptmcmc_ms_cpl_dipol_fixslope_20_nf_set_x_1_ephem_0_20201117.sh</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>/fred/oz002/bgoncharov/correlated_noise_pta_2020_out/dr2_timing_20200607/20200908_20201020_jup_el_5_x1psr/completed.txt</t>
+          <t>/fred/oz002/bgoncharov/correlated_noise_pta_2020_out/dr2_timing_20200607/20200910_cpl_fixgam_20_nf_20201117_dipol_fixgamma_20_nf_x1psr/completed.txt</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>ppta_ptmcmc_ms_cpl_varslope_5_nf_set_x_1_ephem_0</t>
+          <t>ppta_ptmcmc_ms_dip_cpl_fixslope_set_3_1_ephem_0</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>/home/bgonchar/correlated_noise_pta_2020/slurm/ppta_dr2_ptmcmc_ms_cpl_varslope_5_nf_set_x_1_ephem_0_20200928.sh</t>
+          <t>/home/bgonchar/correlated_noise_pta_2020/slurm/ppta_dr2_ptmcmc_ms_cpl_dipol_fixslope_set_3_1_ephem_0_20201121.sh</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>/fred/oz002/bgoncharov/correlated_noise_pta_2020_out/dr2_timing_20200607/20200908_20201021_cpl_vargam_5_nf_x1psr/completed.txt</t>
+          <t>/fred/oz002/bgoncharov/correlated_noise_pta_2020_out/dr2_timing_20200607/20200910_cpl_fixgam_20201103_dipol_fixgamma_3psr/completed.txt</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>ppta_ptmcmc_ms_monop_fixslope_set_x_1_ephem_0</t>
+          <t>ppta_ptmcmc_ms_hdip_cpl_fixsl_20nf_set_x1</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>/home/bgonchar/correlated_noise_pta_2020/slurm/ppta_dr2_ptmcmc_ms_monop_fixslope_set_x_1_ephem_0_20201021.sh</t>
+          <t>/home/bgonchar/correlated_noise_pta_2020/slurm/ppta_dr2_ptmcmc_ms_cpl_halfdip_fixslope_20_nf_set_x_1_20201121.sh</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>/fred/oz002/bgoncharov/correlated_noise_pta_2020_out/dr2_timing_20200607/20200908_20200908_monop_fixgamma_x1psr/completed.txt</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>ppta_ptmcmc_pe_set_x_1_ephem_jup_el_framedr</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>/home/bgonchar/correlated_noise_pta_2020/slurm/ppta_dr2_ptmcmc_pe_set_x_1_ephem_jup_el_fd_20201021.sh</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>/fred/oz002/bgoncharov/correlated_noise_pta_2020_out/dr2_timing_20200607/20200930_be_jup_el_framedr_x1psr/completed.txt</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>ppta_ptmcmc_pe_set_x_1_ephem_mar_el</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>/home/bgonchar/correlated_noise_pta_2020/slurm/ppta_dr2_ptmcmc_pe_set_x_1_ephem_mar_el_20201021.sh</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>/fred/oz002/bgoncharov/correlated_noise_pta_2020_out/dr2_timing_20200607/20200930_be_mar_el_x1psr/completed.txt</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>ppta_ptmcmc_pe_set_x_1_ephem_mer_el</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>/home/bgonchar/correlated_noise_pta_2020/slurm/ppta_dr2_ptmcmc_pe_set_x_1_ephem_mer_el_20201021.sh</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>/fred/oz002/bgoncharov/correlated_noise_pta_2020_out/dr2_timing_20200607/20200930_be_mer_el_x1psr/completed.txt</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>ppta_ptmcmc_pe_set_x_1_ephem_nep_el</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>/home/bgonchar/correlated_noise_pta_2020/slurm/ppta_dr2_ptmcmc_pe_set_x_1_ephem_nep_el_20201021.sh</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>/fred/oz002/bgoncharov/correlated_noise_pta_2020_out/dr2_timing_20200607/20200930_be_nep_el_x1psr/completed.txt</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>ppta_ptmcmc_pe_set_x_1_ephem_sat_el</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>/home/bgonchar/correlated_noise_pta_2020/slurm/ppta_dr2_ptmcmc_pe_set_x_1_ephem_sat_el_20201021.sh</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>/fred/oz002/bgoncharov/correlated_noise_pta_2020_out/dr2_timing_20200607/20200930_be_sat_el_x1psr/completed.txt</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>ppta_ptmcmc_pe_set_x_1_ephem_ura_el</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>/home/bgonchar/correlated_noise_pta_2020/slurm/ppta_dr2_ptmcmc_pe_set_x_1_ephem_ura_el_20201021.sh</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>/fred/oz002/bgoncharov/correlated_noise_pta_2020_out/dr2_timing_20200607/20200930_be_ura_el_x1psr/completed.txt</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>ppta_ptmcmc_pe_set_x_1_ephem_ven_el</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>/home/bgonchar/correlated_noise_pta_2020/slurm/ppta_dr2_ptmcmc_pe_set_x_1_ephem_ven_el_20201021.sh</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>/fred/oz002/bgoncharov/correlated_noise_pta_2020_out/dr2_timing_20200607/20200930_be_ven_el_x1psr/completed.txt</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>ppta_ptmcmc_pe</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>/home/bgonchar/correlated_noise_pta_2020/slurm/ppta_dr2_ptmcmc_pe_h_20200910.sh</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>/fred/oz002/bgoncharov/correlated_noise_pta_2020_out/dr2_timing_20200607/20200908_v1/0_J0437-4715/completed.txt</t>
+          <t>/fred/oz002/bgoncharov/correlated_noise_pta_2020_out/dr2_timing_20200607/20200910_cpl_fixgam_20_nf_20201121_halfdip_fixgamma_20_nf_x1psr/completed.txt</t>
         </is>
       </c>
     </row>

</xml_diff>